<commit_message>
completed parser for run record file
</commit_message>
<xml_diff>
--- a/pyst_developmentPlan.xlsx
+++ b/pyst_developmentPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="26835" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="26835" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="75">
   <si>
     <t>pst</t>
   </si>
@@ -220,6 +220,27 @@
   </si>
   <si>
     <t>FePyST Module</t>
+  </si>
+  <si>
+    <t>dd-correct</t>
+  </si>
+  <si>
+    <t>PEST control file: parameter group section</t>
+  </si>
+  <si>
+    <t>BeoJACTEST, BeoSensan</t>
+  </si>
+  <si>
+    <t>JACTEST results file</t>
+  </si>
+  <si>
+    <t>Run Record file</t>
+  </si>
+  <si>
+    <t>Parameter Value file</t>
+  </si>
+  <si>
+    <t>block separation</t>
   </si>
 </sst>
 </file>
@@ -586,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,7 +651,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -644,13 +665,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -658,111 +679,111 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E11" s="2"/>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="2">
-        <v>0</v>
-      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
@@ -776,51 +797,51 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E22" s="2">
-        <f>E8</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E23" s="2">
         <f>E9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E24" s="2">
-        <v>0</v>
+        <f>E10</f>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>27</v>
@@ -834,7 +855,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
@@ -846,39 +867,50 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>65</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>4</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E32" s="2"/>
+      <c r="E32" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" s="2"/>
@@ -886,8 +918,20 @@
     <row r="34" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E34" s="2"/>
     </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="2"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E7">
+  <conditionalFormatting sqref="E8">
+    <cfRule type="iconSet" priority="11">
+      <iconSet>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0.33"/>
+        <cfvo type="num" val="0.66"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9:E13">
     <cfRule type="iconSet" priority="9">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -896,7 +940,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8:E12">
+  <conditionalFormatting sqref="E19">
     <cfRule type="iconSet" priority="7">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -905,7 +949,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
+  <conditionalFormatting sqref="E21:E27">
     <cfRule type="iconSet" priority="5">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -914,7 +958,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E20:E26">
+  <conditionalFormatting sqref="E29:E35">
     <cfRule type="iconSet" priority="3">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -923,7 +967,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28:E34">
+  <conditionalFormatting sqref="E7">
     <cfRule type="iconSet" priority="1">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -937,7 +981,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="15" id="{124AE956-6B3B-481E-ADFF-F36E65C82696}">
+          <x14:cfRule type="iconSet" priority="17" id="{124AE956-6B3B-481E-ADFF-F36E65C82696}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -953,10 +997,48 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>E7</xm:sqref>
+          <xm:sqref>E8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="16" id="{4E0485F5-F4F3-4C96-BCCE-2380849A8669}">
+          <x14:cfRule type="iconSet" priority="18" id="{4E0485F5-F4F3-4C96-BCCE-2380849A8669}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>E20</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="10" id="{8E388314-5E07-4798-A302-5C50145A1BD5}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>E9:E13</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="8" id="{D13EEFB6-6BAD-4E78-8995-FD61FFCF0BB4}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -975,7 +1057,7 @@
           <xm:sqref>E19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="8" id="{8E388314-5E07-4798-A302-5C50145A1BD5}">
+          <x14:cfRule type="iconSet" priority="6" id="{1EB3ECF8-8FF6-4C0B-B5BE-F2274AF115F1}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -991,10 +1073,10 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>E8:E12</xm:sqref>
+          <xm:sqref>E21:E27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="6" id="{D13EEFB6-6BAD-4E78-8995-FD61FFCF0BB4}">
+          <x14:cfRule type="iconSet" priority="4" id="{829D73C9-4F80-4D32-AD74-4A140C1A4A50}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -1010,10 +1092,10 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>E18</xm:sqref>
+          <xm:sqref>E29:E35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="4" id="{1EB3ECF8-8FF6-4C0B-B5BE-F2274AF115F1}">
+          <x14:cfRule type="iconSet" priority="2" id="{919928BC-91F2-4CCB-95F0-2C9A70962AAC}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -1029,26 +1111,7 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>E20:E26</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{829D73C9-4F80-4D32-AD74-4A140C1A4A50}">
-            <x14:iconSet custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent">
-                <xm:f>33</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent">
-                <xm:f>67</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="1"/>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>E28:E34</xm:sqref>
+          <xm:sqref>E7</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1058,29 +1121,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
     <col min="2" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>55</v>
       </c>
@@ -1093,8 +1157,11 @@
       <c r="D5" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1102,38 +1169,76 @@
         <v>0</v>
       </c>
       <c r="C6" s="2">
-        <f>AVERAGE('PST file'!B5:B21)</f>
+        <f>AVERAGE('PST file'!B7:B23)</f>
         <v>8.8235294117647065E-2</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>55</v>
       </c>
@@ -1147,7 +1252,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -1158,8 +1263,11 @@
         <v>1</v>
       </c>
       <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -1170,8 +1278,11 @@
       <c r="D16" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -1182,24 +1293,27 @@
         <v>1</v>
       </c>
       <c r="D17" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
@@ -1278,10 +1392,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,34 +1423,26 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="B5" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2">
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="2">
         <v>0</v>
@@ -1344,7 +1450,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B9" s="2">
         <v>0</v>
@@ -1352,7 +1458,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -1360,7 +1466,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B11" s="2">
         <v>0</v>
@@ -1368,7 +1474,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B12" s="2">
         <v>0</v>
@@ -1376,7 +1482,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
@@ -1384,18 +1490,15 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B15" s="2">
         <v>0</v>
@@ -1403,45 +1506,48 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B18" s="2">
         <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B19" s="2">
         <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
@@ -1449,15 +1555,31 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B23" s="2">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B5">
-    <cfRule type="iconSet" priority="25">
+  <conditionalFormatting sqref="B7">
+    <cfRule type="iconSet" priority="33">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0.33"/>
@@ -1465,7 +1587,32 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:B21">
+  <conditionalFormatting sqref="B8:B23">
+    <cfRule type="iconSet" priority="12">
+      <iconSet>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0.33"/>
+        <cfvo type="num" val="0.66"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:B23">
+    <cfRule type="iconSet" priority="9">
+      <iconSet>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="10">
+      <iconSet>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="formula" val="0.66"/>
+        <cfvo type="num" val="0.66"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
     <cfRule type="iconSet" priority="4">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -1474,7 +1621,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:B21">
+  <conditionalFormatting sqref="B5">
     <cfRule type="iconSet" priority="1">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -1495,7 +1642,45 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="23" id="{E020DF46-23E3-4D12-B9F4-357E5A0831CC}">
+          <x14:cfRule type="iconSet" priority="31" id="{E020DF46-23E3-4D12-B9F4-357E5A0831CC}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="11" id="{B58AF054-26A1-4C59-BADA-6369A4CAF3F6}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B8:B23</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="3" id="{C65A0D50-6CF4-406D-8937-94093C87594C}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -1513,25 +1698,6 @@
           </x14:cfRule>
           <xm:sqref>B5</xm:sqref>
         </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="3" id="{B58AF054-26A1-4C59-BADA-6369A4CAF3F6}">
-            <x14:iconSet custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent">
-                <xm:f>33</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent">
-                <xm:f>67</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="1"/>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>B6:B21</xm:sqref>
-        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
pest control file object now support observation groups and parameter groups
</commit_message>
<xml_diff>
--- a/pyst_developmentPlan.xlsx
+++ b/pyst_developmentPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="26835" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="26835" windowHeight="12525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
   <si>
     <t>pst</t>
   </si>
@@ -1126,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="C6" s="2">
         <f>AVERAGE('PST file'!B7:B23)</f>
-        <v>8.8235294117647065E-2</v>
+        <v>0.29411764705882354</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -1397,8 +1397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,7 +1429,7 @@
         <v>74</v>
       </c>
       <c r="B5" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>75</v>
@@ -1440,7 +1440,7 @@
         <v>34</v>
       </c>
       <c r="B7" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -1491,7 +1491,10 @@
         <v>36</v>
       </c>
       <c r="B13" s="2">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1499,7 +1502,10 @@
         <v>37</v>
       </c>
       <c r="B14" s="2">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1507,7 +1513,7 @@
         <v>38</v>
       </c>
       <c r="B15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added support to write uncertainty files (unc)
</commit_message>
<xml_diff>
--- a/pyst_developmentPlan.xlsx
+++ b/pyst_developmentPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="26835" windowHeight="12525" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="25905" windowHeight="10230" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="102">
   <si>
     <t>pst</t>
   </si>
@@ -246,9 +246,6 @@
     <t>PyST.feflow Package</t>
   </si>
   <si>
-    <t>ProxyModel</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -- general --</t>
   </si>
   <si>
@@ -304,6 +301,27 @@
   </si>
   <si>
     <t>[various]</t>
+  </si>
+  <si>
+    <t>ProxyModel, Monte-Carlo simulation</t>
+  </si>
+  <si>
+    <t>ASCII table file</t>
+  </si>
+  <si>
+    <t>Covariance File</t>
+  </si>
+  <si>
+    <t>cited in UNC file</t>
+  </si>
+  <si>
+    <t>matrix file</t>
+  </si>
+  <si>
+    <t>mat</t>
+  </si>
+  <si>
+    <t>BeoJACTEST, BeoSENSAN</t>
   </si>
 </sst>
 </file>
@@ -804,7 +822,7 @@
         <v>0.9</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -986,22 +1004,22 @@
         <v>9</v>
       </c>
       <c r="D32" s="2">
-        <f>ParserWriter!D12</f>
-        <v>0</v>
+        <f>ParserWriter!D13</f>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" t="s">
         <v>90</v>
-      </c>
-      <c r="B33" t="s">
-        <v>91</v>
       </c>
       <c r="C33" t="s">
         <v>10</v>
       </c>
       <c r="D33" s="2">
-        <f>ParserWriter!D13</f>
+        <f>ParserWriter!D15</f>
         <v>0</v>
       </c>
     </row>
@@ -1013,53 +1031,53 @@
     </row>
     <row r="36" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C37" t="s">
         <v>10</v>
       </c>
       <c r="D37" s="2">
-        <f>ParserWriter!C31</f>
+        <f>ParserWriter!C29</f>
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C38" t="s">
         <v>10</v>
       </c>
       <c r="D38" s="2">
-        <f>ParserWriter!C29</f>
+        <f>ParserWriter!C27</f>
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C39" t="s">
         <v>9</v>
       </c>
       <c r="D39" s="2">
-        <f>ParserWriter!D29</f>
+        <f>ParserWriter!D27</f>
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D42" s="2">
         <v>1</v>
@@ -1067,7 +1085,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D43" s="2">
         <v>0</v>
@@ -1075,7 +1093,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D44" s="2">
         <v>0</v>
@@ -1083,7 +1101,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D45" s="2">
         <v>0</v>
@@ -1091,7 +1109,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D46" s="2">
         <v>0</v>
@@ -1409,17 +1427,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
@@ -1451,10 +1469,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
@@ -1465,7 +1483,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -1478,7 +1496,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1498,99 +1516,97 @@
         <v>65</v>
       </c>
       <c r="F8" t="s">
-        <v>94</v>
-      </c>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2"/>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2">
-        <v>1</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2"/>
       <c r="E11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" t="s">
         <v>78</v>
       </c>
-      <c r="B13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s">
-        <v>13</v>
-      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C16" s="2">
         <v>0</v>
@@ -1604,7 +1620,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C17" s="2">
         <v>0</v>
@@ -1618,7 +1634,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="2">
         <v>0</v>
@@ -1632,7 +1648,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="2">
         <v>0</v>
@@ -1644,91 +1660,111 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>56</v>
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="C29" s="2">
         <v>1</v>
       </c>
-      <c r="D29" s="2">
-        <v>1</v>
-      </c>
+      <c r="D29" s="2"/>
       <c r="E29" t="s">
         <v>63</v>
       </c>
-      <c r="F29" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2">
-        <v>1</v>
-      </c>
-      <c r="E30" t="s">
-        <v>63</v>
-      </c>
-      <c r="F30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="2">
-        <v>1</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" t="s">
-        <v>63</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C29:D31">
-    <cfRule type="iconSet" priority="32">
+  <conditionalFormatting sqref="C27:D29">
+    <cfRule type="iconSet" priority="37">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1736,8 +1772,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6 C13:C19">
-    <cfRule type="iconSet" priority="123">
+  <conditionalFormatting sqref="C27:D29 C11:D13 C7:D9 C22:D23 D6 D14:D21">
+    <cfRule type="iconSet" priority="137">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1745,8 +1781,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6 C13:C19">
-    <cfRule type="iconSet" priority="125">
+  <conditionalFormatting sqref="C27:D29 C11:D13 C7:D9 C22:D23 D6 D14:D21">
+    <cfRule type="iconSet" priority="143">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0.33"/>
@@ -1754,15 +1790,15 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6 C13:C19">
-    <cfRule type="iconSet" priority="127">
+  <conditionalFormatting sqref="C27:D29 C11:D13 C7:D9 C22:D23 D6 D14:D21">
+    <cfRule type="iconSet" priority="149">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
         <cfvo type="percent" val="67"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="128">
+    <cfRule type="iconSet" priority="150">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="formula" val="0.66"/>
@@ -1770,8 +1806,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:D12 C7:D8 C23:D25 C29:D31 D6 D13:D19">
-    <cfRule type="iconSet" priority="132">
+  <conditionalFormatting sqref="C15:C21 C6">
+    <cfRule type="iconSet" priority="162">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1779,8 +1815,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:D12 C7:D8 C23:D25 C29:D31 D6 D13:D19">
-    <cfRule type="iconSet" priority="138">
+  <conditionalFormatting sqref="C15:C21 C6">
+    <cfRule type="iconSet" priority="165">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0.33"/>
@@ -1788,15 +1824,15 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:D12 C7:D8 C23:D25 C29:D31 D6 D13:D19">
-    <cfRule type="iconSet" priority="144">
+  <conditionalFormatting sqref="C15:C21 C6">
+    <cfRule type="iconSet" priority="168">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
         <cfvo type="percent" val="67"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="145">
+    <cfRule type="iconSet" priority="169">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="formula" val="0.66"/>
@@ -1809,7 +1845,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="131" id="{9C00AC43-648D-4B27-95C3-36469AF4F171}">
+          <x14:cfRule type="iconSet" priority="161" id="{4DDF3C13-97DD-41FF-95BB-70B14AAB1425}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -1825,10 +1861,10 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>C6 C13:C19</xm:sqref>
+          <xm:sqref>C27:D29 C11:D13 C7:D9 C22:D23 D6 D14:D21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="156" id="{4DDF3C13-97DD-41FF-95BB-70B14AAB1425}">
+          <x14:cfRule type="iconSet" priority="198" id="{9C00AC43-648D-4B27-95C3-36469AF4F171}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -1844,7 +1880,7 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>C10:D12 C7:D8 C23:D25 C29:D31 D6 D13:D19</xm:sqref>
+          <xm:sqref>C15:C21 C6</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1856,7 +1892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added basic parser for run management record file
</commit_message>
<xml_diff>
--- a/pyst_developmentPlan.xlsx
+++ b/pyst_developmentPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="25905" windowHeight="10230" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="25905" windowHeight="10230" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="106">
   <si>
     <t>pst</t>
   </si>
@@ -328,6 +328,12 @@
   </si>
   <si>
     <t>relative-datum (corrector)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run management record </t>
+  </si>
+  <si>
+    <t>rmr</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1054,7 @@
         <v>10</v>
       </c>
       <c r="D37" s="2">
-        <f>ParserWriter!C29</f>
+        <f>ParserWriter!C30</f>
         <v>1</v>
       </c>
     </row>
@@ -1060,7 +1066,7 @@
         <v>10</v>
       </c>
       <c r="D38" s="2">
-        <f>ParserWriter!C27</f>
+        <f>ParserWriter!C28</f>
         <v>1</v>
       </c>
     </row>
@@ -1072,7 +1078,7 @@
         <v>9</v>
       </c>
       <c r="D39" s="2">
-        <f>ParserWriter!D27</f>
+        <f>ParserWriter!D28</f>
         <v>1</v>
       </c>
     </row>
@@ -1433,10 +1439,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,58 +1697,48 @@
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C22" s="2"/>
+      <c r="A22" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+    <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="2">
-        <v>1</v>
-      </c>
-      <c r="D27" s="2">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
       <c r="D28" s="2">
         <v>1</v>
       </c>
@@ -1750,40 +1746,58 @@
         <v>62</v>
       </c>
       <c r="F28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="2">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2">
+        <v>1</v>
+      </c>
       <c r="E29" t="s">
         <v>62</v>
       </c>
+      <c r="F29" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B30" t="s">
         <v>26</v>
       </c>
       <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="2">
         <v>0.25</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>102</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C27:D29 C30">
+  <conditionalFormatting sqref="C28:D30 C31">
     <cfRule type="iconSet" priority="37">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -1792,7 +1806,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27:D29 C11:D13 C7:D9 C22:D23 D6 D14:D21 C30">
+  <conditionalFormatting sqref="C28:D30 C11:D13 C7:D9 C24:D24 D6 D14:D21 C31 C22:D22">
     <cfRule type="iconSet" priority="137">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -1801,7 +1815,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27:D29 C11:D13 C7:D9 C22:D23 D6 D14:D21 C30">
+  <conditionalFormatting sqref="C28:D30 C11:D13 C7:D9 C24:D24 D6 D14:D21 C31 C22:D22">
     <cfRule type="iconSet" priority="143">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -1810,7 +1824,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27:D29 C11:D13 C7:D9 C22:D23 D6 D14:D21 C30">
+  <conditionalFormatting sqref="C28:D30 C11:D13 C7:D9 C24:D24 D6 D14:D21 C31 C22:D22">
     <cfRule type="iconSet" priority="149">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -1881,7 +1895,7 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>C27:D29 C11:D13 C7:D9 C22:D23 D6 D14:D21 C30</xm:sqref>
+          <xm:sqref>C28:D30 C11:D13 C7:D9 C24:D24 D6 D14:D21 C31 C22:D22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="198" id="{9C00AC43-648D-4B27-95C3-36469AF4F171}">
@@ -1912,7 +1926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added first version of Prior Information Dashboard
</commit_message>
<xml_diff>
--- a/pyst_developmentPlan.xlsx
+++ b/pyst_developmentPlan.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\red5alex.cloudforge\pyst\trunk\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="25905" windowHeight="10230" activeTab="1"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="ParserWriter" sheetId="3" r:id="rId2"/>
     <sheet name="PST file" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="108">
   <si>
     <t>pst</t>
   </si>
@@ -334,6 +339,12 @@
   </si>
   <si>
     <t>rmr</t>
+  </si>
+  <si>
+    <t>PI Dashboard</t>
+  </si>
+  <si>
+    <t>BeoSENSAN, PI Dashboard</t>
   </si>
 </sst>
 </file>
@@ -419,6 +430,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -466,7 +480,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -501,7 +515,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1016,7 +1030,7 @@
         <v>9</v>
       </c>
       <c r="D32" s="2">
-        <f>ParserWriter!D13</f>
+        <f>ParserWriter!E13</f>
         <v>1</v>
       </c>
     </row>
@@ -1031,7 +1045,7 @@
         <v>10</v>
       </c>
       <c r="D33" s="2">
-        <f>ParserWriter!D15</f>
+        <f>ParserWriter!E15</f>
         <v>0</v>
       </c>
     </row>
@@ -1078,7 +1092,7 @@
         <v>9</v>
       </c>
       <c r="D39" s="2">
-        <f>ParserWriter!D28</f>
+        <f>ParserWriter!E28</f>
         <v>1</v>
       </c>
     </row>
@@ -1439,30 +1453,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>54</v>
       </c>
@@ -1473,13 +1488,16 @@
         <v>55</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>90</v>
       </c>
@@ -1489,11 +1507,12 @@
       <c r="C6" s="7">
         <v>1</v>
       </c>
-      <c r="D6" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>89</v>
       </c>
@@ -1504,14 +1523,15 @@
         <f>AVERAGE('PST file'!B7:B23)</f>
         <v>0.29411764705882354</v>
       </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>66</v>
       </c>
@@ -1521,33 +1541,35 @@
       <c r="C8" s="2">
         <v>1</v>
       </c>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
         <v>64</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>94</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>65</v>
       </c>
@@ -1558,11 +1580,12 @@
         <v>1</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" t="s">
+      <c r="E11" s="2"/>
+      <c r="F11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>67</v>
       </c>
@@ -1570,14 +1593,15 @@
         <v>2</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>61</v>
       </c>
@@ -1585,28 +1609,29 @@
         <v>4</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="2">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>95</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>76</v>
       </c>
@@ -1615,78 +1640,94 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="2">
         <v>0</v>
       </c>
-      <c r="D16" s="2">
-        <v>0</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="2">
         <v>0</v>
       </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="2">
         <v>0</v>
       </c>
-      <c r="D18" s="2">
-        <v>0</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="2">
         <v>0</v>
       </c>
-      <c r="D19" s="2">
-        <v>0</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="D19" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="2">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0</v>
-      </c>
-      <c r="E20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>97</v>
       </c>
@@ -1695,8 +1736,9 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>104</v>
       </c>
@@ -1707,15 +1749,17 @@
         <v>1</v>
       </c>
       <c r="D22" s="2"/>
-    </row>
-    <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E22" s="2"/>
+    </row>
+    <row r="24" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E24" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -1725,11 +1769,12 @@
       <c r="C26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -1739,17 +1784,18 @@
       <c r="C28" s="2">
         <v>1</v>
       </c>
-      <c r="D28" s="2">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="D28" s="2"/>
+      <c r="E28" s="2">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
         <v>62</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>71</v>
       </c>
@@ -1757,17 +1803,18 @@
         <v>58</v>
       </c>
       <c r="C29" s="2"/>
-      <c r="D29" s="2">
-        <v>1</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="D29" s="2"/>
+      <c r="E29" s="2">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
         <v>62</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>100</v>
       </c>
@@ -1778,11 +1825,12 @@
         <v>1</v>
       </c>
       <c r="D30" s="2"/>
-      <c r="E30" t="s">
+      <c r="E30" s="2"/>
+      <c r="F30" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>101</v>
       </c>
@@ -1792,12 +1840,13 @@
       <c r="C31" s="2">
         <v>0.25</v>
       </c>
-      <c r="E31" t="s">
+      <c r="D31" s="2"/>
+      <c r="F31" t="s">
         <v>102</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C28:D30 C31">
+  <conditionalFormatting sqref="C28:E30 C31:D31">
     <cfRule type="iconSet" priority="37">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -1806,7 +1855,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:D30 C11:D13 C7:D9 C24:D24 D6 D14:D21 C31 C22:D22">
+  <conditionalFormatting sqref="C28:E30 C11:E13 C7:E9 C24:E24 E6 E14:E21 C31:D31 C22:E22">
     <cfRule type="iconSet" priority="137">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -1815,7 +1864,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:D30 C11:D13 C7:D9 C24:D24 D6 D14:D21 C31 C22:D22">
+  <conditionalFormatting sqref="C28:E30 C11:E13 C7:E9 C24:E24 E6 E14:E21 C31:D31 C22:E22">
     <cfRule type="iconSet" priority="143">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -1824,7 +1873,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:D30 C11:D13 C7:D9 C24:D24 D6 D14:D21 C31 C22:D22">
+  <conditionalFormatting sqref="C28:E30 C11:E13 C7:E9 C24:E24 E6 E14:E21 C31:D31 C22:E22">
     <cfRule type="iconSet" priority="149">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -1840,7 +1889,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:C21 C6">
+  <conditionalFormatting sqref="C15:D15 C6:D6 C20:D21 C16:C19">
     <cfRule type="iconSet" priority="162">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -1849,7 +1898,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:C21 C6">
+  <conditionalFormatting sqref="C15:D15 C6:D6 C20:D21 C16:C19">
     <cfRule type="iconSet" priority="165">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -1858,7 +1907,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:C21 C6">
+  <conditionalFormatting sqref="C15:D15 C6:D6 C20:D21 C16:C19">
     <cfRule type="iconSet" priority="168">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -1895,7 +1944,7 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>C28:D30 C11:D13 C7:D9 C24:D24 D6 D14:D21 C31 C22:D22</xm:sqref>
+          <xm:sqref>C28:E30 C11:E13 C7:E9 C24:E24 E6 E14:E21 C31:D31 C22:E22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="198" id="{9C00AC43-648D-4B27-95C3-36469AF4F171}">
@@ -1914,7 +1963,7 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>C15:C21 C6</xm:sqref>
+          <xm:sqref>C15:D15 C6:D6 C20:D21 C16:C19</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1927,7 +1976,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2093,6 +2142,9 @@
       <c r="B20" s="2">
         <v>0</v>
       </c>
+      <c r="C20" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">

</xml_diff>